<commit_message>
Update The Black Vault File Dump Open Directories.xlsx
</commit_message>
<xml_diff>
--- a/Assests/The Black Vault File Dump Open Directories.xlsx
+++ b/Assests/The Black Vault File Dump Open Directories.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="28770" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="28770" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Main Directories" sheetId="1" r:id="rId1"/>
     <sheet name="Other Files" sheetId="3" r:id="rId2"/>
     <sheet name="Unexplored" sheetId="2" r:id="rId3"/>
+    <sheet name="Book Marks" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="255">
   <si>
     <t>The Black Vault File Dump Open Directories</t>
   </si>
@@ -748,6 +749,39 @@
   </si>
   <si>
     <t>left off here</t>
+  </si>
+  <si>
+    <t>https://documents.theblackvault.com/documents/eeoc/</t>
+  </si>
+  <si>
+    <t>https://documents.theblackvault.com/documents/commercedept/</t>
+  </si>
+  <si>
+    <t>https://documents.theblackvault.com/documents/usaf/</t>
+  </si>
+  <si>
+    <t>https://documents.theblackvault.com/documents/federalreserve/</t>
+  </si>
+  <si>
+    <t>https://documents.theblackvault.com/documents/travelexpenditures/</t>
+  </si>
+  <si>
+    <t>https://documents.theblackvault.com/documents/rrb/</t>
+  </si>
+  <si>
+    <t>https://documents.theblackvault.com/documents/dea/</t>
+  </si>
+  <si>
+    <t>https://documents.theblackvault.com/documents/megabyteact/</t>
+  </si>
+  <si>
+    <t>https://documents.theblackvault.com/documents/smithsonian/</t>
+  </si>
+  <si>
+    <t>https://documents.theblackvault.com/documents/ODNI/</t>
+  </si>
+  <si>
+    <t>January 16th, 2021</t>
   </si>
 </sst>
 </file>
@@ -826,7 +860,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
@@ -841,9 +875,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1152,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D144"/>
+  <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I114" sqref="I114"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,6 +1946,59 @@
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C144" t="s">
         <v>241</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B146" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>226</v>
+      </c>
+      <c r="B155" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -1935,9 +2019,10 @@
     <hyperlink ref="C39" r:id="rId14"/>
     <hyperlink ref="B91" r:id="rId15"/>
     <hyperlink ref="C92" r:id="rId16"/>
+    <hyperlink ref="B146" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -1946,7 +2031,7 @@
   <dimension ref="A2:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2032,60 +2117,54 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>242</v>
-      </c>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>243</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A26" r:id="rId1" display="https://www.theblackvault.com/documentarchive/revised-acquisition-program-baseline-threat-assessment-chemical-demilitarization-program-october-2002/"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2093,8 +2172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:N1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2612,4 +2691,33 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.theblackvault.com/documentarchive/revised-acquisition-program-baseline-threat-assessment-chemical-demilitarization-program-october-2002/"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>